<commit_message>
Update no bom do painel (código correto do conector Axonn).
</commit_message>
<xml_diff>
--- a/HW_Design/fontes_projetos/painel_meb_1_02/pim_painel_meb/bom/painel_meb_1_02_bom.xlsx
+++ b/HW_Design/fontes_projetos/painel_meb_1_02/pim_painel_meb/bom/painel_meb_1_02_bom.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\nsee\citar_simucam\hw\pim_painel_meb\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cassio\repo_simucam\SimuCam_Development\HW_Design\fontes_projetos\painel_meb_1_02\pim_painel_meb\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="11268"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="11265"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-painel_meb" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="115">
   <si>
     <t>Quantity</t>
   </si>
@@ -266,9 +266,6 @@
     <t>Axonn</t>
   </si>
   <si>
-    <t>MSAP102SBS1G2G02L2E</t>
-  </si>
-  <si>
     <t>Header, 2-Pin - duas travas laterais</t>
   </si>
   <si>
@@ -365,13 +362,7 @@
     <t>RC0603JR-0710KL</t>
   </si>
   <si>
-    <t>Quantidade para 5 placas</t>
-  </si>
-  <si>
     <t>MSAP102SBS1G2GCEL2E</t>
-  </si>
-  <si>
-    <t>Part number corrigido:</t>
   </si>
   <si>
     <t>R50</t>
@@ -409,8 +400,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -478,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -510,17 +503,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -806,32 +796,31 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="41.109375" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" customWidth="1"/>
-    <col min="10" max="10" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -845,7 +834,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
@@ -854,16 +843,11 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -874,10 +858,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>9</v>
@@ -886,10 +870,11 @@
         <v>2</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -900,10 +885,10 @@
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
@@ -912,10 +897,11 @@
         <v>2</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -926,10 +912,10 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>9</v>
@@ -938,10 +924,11 @@
         <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -952,10 +939,10 @@
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>9</v>
@@ -964,10 +951,11 @@
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -978,10 +966,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>19</v>
@@ -990,10 +978,11 @@
         <v>2</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>77</v>
       </c>
@@ -1001,13 +990,13 @@
         <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>20</v>
@@ -1018,8 +1007,9 @@
       <c r="H9" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>78</v>
       </c>
@@ -1027,13 +1017,13 @@
         <v>79</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="E10" s="9" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>20</v>
@@ -1044,15 +1034,9 @@
       <c r="H10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I10" s="12">
-        <f>(5*G10)</f>
-        <v>10</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1066,7 +1050,7 @@
         <v>23</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>24</v>
@@ -1078,7 +1062,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>72</v>
       </c>
@@ -1092,7 +1076,7 @@
         <v>73</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>72</v>
@@ -1101,10 +1085,10 @@
         <v>1</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -1118,7 +1102,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>28</v>
@@ -1130,7 +1114,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
@@ -1153,10 +1137,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
@@ -1179,10 +1163,10 @@
         <v>8</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="34.200000000000003" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
@@ -1205,10 +1189,10 @@
         <v>21</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>43</v>
       </c>
@@ -1219,10 +1203,10 @@
         <v>44</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>45</v>
@@ -1231,10 +1215,10 @@
         <v>3</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="34.200000000000003" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>47</v>
       </c>
@@ -1245,10 +1229,10 @@
         <v>48</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>45</v>
@@ -1257,10 +1241,10 @@
         <v>21</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="34.200000000000003" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>49</v>
       </c>
@@ -1271,10 +1255,10 @@
         <v>50</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>45</v>
@@ -1283,10 +1267,10 @@
         <v>21</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>51</v>
       </c>
@@ -1297,10 +1281,10 @@
         <v>52</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>45</v>
@@ -1309,12 +1293,12 @@
         <v>3</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>46</v>
@@ -1323,10 +1307,10 @@
         <v>53</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>45</v>
@@ -1335,13 +1319,13 @@
         <v>1</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>54</v>
       </c>
@@ -1367,7 +1351,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>58</v>
       </c>
@@ -1393,7 +1377,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>62</v>
       </c>
@@ -1407,7 +1391,7 @@
         <v>63</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>65</v>
@@ -1416,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>